<commit_message>
fixed bug with RR stage and immediates
</commit_message>
<xml_diff>
--- a/TACKY.xlsx
+++ b/TACKY.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="149">
   <si>
     <t xml:space="preserve">Macro</t>
   </si>
@@ -400,37 +400,34 @@
     <t xml:space="preserve">Store</t>
   </si>
   <si>
+    <t xml:space="preserve">a2r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reg. Swap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">li</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arithmetic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slt</t>
+  </si>
+  <si>
     <t xml:space="preserve">cvt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conversion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a2r</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reg. Swap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">r2a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">li</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Load</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arithmetic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">slt</t>
   </si>
   <si>
     <t xml:space="preserve">add</t>
@@ -694,11 +691,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -794,16 +791,19 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1325,7 +1325,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1643,12 +1643,10 @@
       <c r="E13" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>126</v>
-      </c>
+      <c r="F13" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="K13" s="12"/>
     </row>
@@ -1669,12 +1667,14 @@
         <v>0</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H14" s="6"/>
+        <v>126</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="n">
@@ -1693,7 +1693,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -1714,11 +1714,11 @@
       <c r="E16" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F16" s="20" t="s">
-        <v>130</v>
+      <c r="F16" s="19" t="s">
+        <v>128</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H16" s="6"/>
     </row>
@@ -1738,8 +1738,8 @@
       <c r="E17" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F17" s="20" t="s">
-        <v>132</v>
+      <c r="F17" s="19" t="s">
+        <v>130</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -1843,11 +1843,11 @@
       <c r="E22" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F22" s="19" t="s">
-        <v>133</v>
+      <c r="F22" s="20" t="s">
+        <v>131</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H22" s="6" t="s">
         <v>122</v>
@@ -1870,8 +1870,8 @@
       <c r="E23" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F23" s="19" t="s">
-        <v>135</v>
+      <c r="F23" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -1914,9 +1914,15 @@
       <c r="E25" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="F25" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="n">
@@ -1934,15 +1940,11 @@
       <c r="E26" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F26" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>122</v>
-      </c>
+      <c r="F26" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="n">
@@ -1960,8 +1962,8 @@
       <c r="E27" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F27" s="19" t="s">
-        <v>137</v>
+      <c r="F27" s="20" t="s">
+        <v>136</v>
       </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
@@ -1982,8 +1984,8 @@
       <c r="E28" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F28" s="19" t="s">
-        <v>138</v>
+      <c r="F28" s="20" t="s">
+        <v>137</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -2004,8 +2006,8 @@
       <c r="E29" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F29" s="19" t="s">
-        <v>139</v>
+      <c r="F29" s="20" t="s">
+        <v>138</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
@@ -2026,11 +2028,11 @@
       <c r="E30" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="G30" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="H30" s="6"/>
     </row>
@@ -2050,8 +2052,8 @@
       <c r="E31" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F31" s="19" t="s">
-        <v>142</v>
+      <c r="F31" s="20" t="s">
+        <v>141</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
@@ -2072,8 +2074,8 @@
       <c r="E32" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F32" s="19" t="s">
-        <v>143</v>
+      <c r="F32" s="20" t="s">
+        <v>142</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
@@ -2094,14 +2096,14 @@
       <c r="E33" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F33" s="19" t="s">
-        <v>144</v>
+      <c r="F33" s="20" t="s">
+        <v>143</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="19">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="F2:H2"/>
@@ -2109,20 +2111,22 @@
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="F10:H10"/>
-    <mergeCell ref="H11:H17"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="F13:H13"/>
     <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H17"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="F18:H21"/>
     <mergeCell ref="G22:G23"/>
     <mergeCell ref="H22:H23"/>
-    <mergeCell ref="F24:H25"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H33"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="G25:G29"/>
+    <mergeCell ref="H25:H33"/>
     <mergeCell ref="G30:G33"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2144,10 +2148,10 @@
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.15"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -2187,11 +2191,11 @@
       <c r="E2" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>140</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>102</v>
@@ -2219,8 +2223,8 @@
       <c r="E3" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>143</v>
+      <c r="F3" s="20" t="s">
+        <v>142</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -2245,8 +2249,8 @@
       <c r="E4" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>144</v>
+      <c r="F4" s="20" t="s">
+        <v>143</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -2271,8 +2275,8 @@
       <c r="E5" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="19" t="s">
-        <v>142</v>
+      <c r="F5" s="20" t="s">
+        <v>141</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -2297,11 +2301,11 @@
       <c r="E6" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>136</v>
+      <c r="F6" s="20" t="s">
+        <v>135</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2322,8 +2326,8 @@
       <c r="E7" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>137</v>
+      <c r="F7" s="20" t="s">
+        <v>136</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -2345,8 +2349,8 @@
       <c r="E8" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>139</v>
+      <c r="F8" s="20" t="s">
+        <v>138</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -2368,8 +2372,8 @@
       <c r="E9" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="19" t="s">
-        <v>138</v>
+      <c r="F9" s="20" t="s">
+        <v>137</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -2391,8 +2395,8 @@
       <c r="E10" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="19" t="s">
-        <v>133</v>
+      <c r="F10" s="20" t="s">
+        <v>131</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -2414,8 +2418,8 @@
       <c r="E11" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>135</v>
+      <c r="F11" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -2437,8 +2441,8 @@
       <c r="E12" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="19" t="s">
-        <v>125</v>
+      <c r="F12" s="20" t="s">
+        <v>134</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -2460,11 +2464,11 @@
       <c r="E13" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="20" t="s">
-        <v>132</v>
+      <c r="F13" s="19" t="s">
+        <v>130</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -2485,8 +2489,8 @@
       <c r="E14" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="20" t="s">
-        <v>130</v>
+      <c r="F14" s="19" t="s">
+        <v>128</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -2532,10 +2536,10 @@
         <v>0</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
@@ -2557,7 +2561,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -2588,7 +2592,7 @@
         <v>121</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I18" s="6"/>
     </row>
@@ -2776,7 +2780,7 @@
         <v>118</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="21"/>
@@ -2936,7 +2940,7 @@
         <v>110</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I33" s="6"/>
     </row>
@@ -2961,7 +2965,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2985,7 +2989,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.68"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.88"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -3025,10 +3029,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>122</v>
@@ -3055,7 +3059,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -3079,8 +3083,8 @@
       <c r="E4" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>136</v>
+      <c r="F4" s="20" t="s">
+        <v>135</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>102</v>
@@ -3106,8 +3110,8 @@
       <c r="E5" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="19" t="s">
-        <v>143</v>
+      <c r="F5" s="20" t="s">
+        <v>142</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -3131,8 +3135,8 @@
       <c r="E6" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="19" t="s">
-        <v>125</v>
+      <c r="F6" s="20" t="s">
+        <v>134</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -3154,8 +3158,8 @@
       <c r="E7" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>138</v>
+      <c r="F7" s="20" t="s">
+        <v>137</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
@@ -3176,8 +3180,8 @@
       <c r="E8" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="19" t="s">
-        <v>139</v>
+      <c r="F8" s="20" t="s">
+        <v>138</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -3198,8 +3202,8 @@
       <c r="E9" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="19" t="s">
-        <v>140</v>
+      <c r="F9" s="20" t="s">
+        <v>139</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -3220,8 +3224,8 @@
       <c r="E10" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="19" t="s">
-        <v>144</v>
+      <c r="F10" s="20" t="s">
+        <v>143</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -3242,8 +3246,8 @@
       <c r="E11" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>133</v>
+      <c r="F11" s="20" t="s">
+        <v>131</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -3264,8 +3268,8 @@
       <c r="E12" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="19" t="s">
-        <v>135</v>
+      <c r="F12" s="20" t="s">
+        <v>133</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -3286,8 +3290,8 @@
       <c r="E13" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="19" t="s">
-        <v>137</v>
+      <c r="F13" s="20" t="s">
+        <v>136</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -3310,8 +3314,8 @@
       <c r="E14" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="19" t="s">
-        <v>142</v>
+      <c r="F14" s="20" t="s">
+        <v>141</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -3422,11 +3426,11 @@
       <c r="E19" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="F19" s="20" t="s">
-        <v>132</v>
+      <c r="F19" s="19" t="s">
+        <v>130</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H19" s="6"/>
       <c r="J19" s="12"/>
@@ -3448,8 +3452,8 @@
       <c r="E20" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="F20" s="20" t="s">
-        <v>130</v>
+      <c r="F20" s="19" t="s">
+        <v>128</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -3579,7 +3583,7 @@
         <v>117</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>107</v>
@@ -3629,7 +3633,7 @@
         <v>116</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H28" s="6"/>
     </row>
@@ -3700,7 +3704,7 @@
         <v>105</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H31" s="6"/>
     </row>
@@ -3767,7 +3771,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>